<commit_message>
Changed location of bInterruptProcess on PLC project and OPC UA server. It is now located in an extra struct. Changed the Datapoints in connection_KEA.json and LogVariablesExperiment.xlsx
</commit_message>
<xml_diff>
--- a/data_logging/LogVariablesExperiment.xlsx
+++ b/data_logging/LogVariablesExperiment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B.Grosch_Lokal\Documents\GitRepositories\cpsl2023-dr-for-cleaning-machines\data_logging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\cpsl2023-dr-for-cleaning-machines\data_logging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C39EF0C-CA73-476C-AAB8-72ECA2928922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C813B1-0A8B-4338-A9C3-48F0EE58CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FE4DFC22-88A4-47D8-A40A-925B06C88741}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE4DFC22-88A4-47D8-A40A-925B06C88741}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="94">
   <si>
     <t>Code</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>PythonCode</t>
+  </si>
+  <si>
+    <t>ns=2;s=Application.Plc_Main.KEA.interruptProcess.bInterruptProcessAlgorithm</t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +965,7 @@
         <v>4840</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1844,15 +1847,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC43C22BD5AB4D438308D6F08CFAB525" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d8997b37f6fdc633bf60fc63e6c3957f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="595ccc5b-7df1-4723-bc2e-56b8b2b49834" xmlns:ns3="5446275f-1b3c-43d4-b9b4-71080fbfb2f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0e3b0aa3656617aa8ed57f2fa04d715" ns2:_="" ns3:_="">
     <xsd:import namespace="595ccc5b-7df1-4723-bc2e-56b8b2b49834"/>
@@ -2061,15 +2055,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6557A8C2-3F38-424B-B9B2-5A74D5B28F56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF09054-62A9-4CA8-B9DA-A8C1201036FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2086,4 +2081,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6557A8C2-3F38-424B-B9B2-5A74D5B28F56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>